<commit_message>
Added Yizhens class to create stat bar output: currently debugging the issue
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\ICDC_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE277DF-2CDB-4DBB-ADAD-CD845B45CDA8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FDA650-7E33-4DD4-9683-562A8CC42451}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>WebExcel</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>TC01_Canine_Filter_Breed-Akita_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Akita']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+  </si>
+  <si>
+    <t>StatQuery</t>
   </si>
 </sst>
 </file>
@@ -419,20 +426,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="75.81640625" customWidth="1"/>
     <col min="2" max="2" width="70.26953125" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" customWidth="1"/>
+    <col min="3" max="3" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -440,10 +448,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -451,6 +462,9 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -459,4 +473,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D94671-34CB-46BD-8964-4DC9A3E8B07A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added switch for ICDC and CTDC case level detail & query for reading case detail table
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D71EFAC-311B-42E8-93AA-2863F83A0D02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B65A803-FAB2-42AC-93A9-603A03431778}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>WebExcel</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>StatQuery</t>
+  </si>
+  <si>
+    <t>caseDetailQuery</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)-[*]-&gt;(c:case) WITH DISTINCT(f) AS f, c MATCH (f)--&gt;(parent) WHERE c.case_id IN ['NCATS-COP01CCB010072'] RETURN f.file_name AS `File Name` ,f.file_type AS `File Type`,head(labels(parent)) AS `Association`, f.file_description AS `Description`,f.file_format AS Format,((f.file_size)/1024) AS Size</t>
   </si>
 </sst>
 </file>
@@ -426,21 +432,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="75.81640625" customWidth="1"/>
     <col min="2" max="2" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="40.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="40.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -448,23 +455,29 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
branched out column count as per application & page
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B65A803-FAB2-42AC-93A9-603A03431778}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE6A4D8-4B0A-469A-AD58-3199608DB243}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
corrected dynamic case id in query for casedetails
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
+++ b/InputFiles/TC01_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE6A4D8-4B0A-469A-AD58-3199608DB243}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BD2BD5-389C-4953-84BF-1C51ED83BDBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>WebExcel</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>StatQuery</t>
-  </si>
-  <si>
-    <t>caseDetailQuery</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)-[*]-&gt;(c:case) WITH DISTINCT(f) AS f, c MATCH (f)--&gt;(parent) WHERE c.case_id IN ['NCATS-COP01CCB010072'] RETURN f.file_name AS `File Name` ,f.file_type AS `File Type`,head(labels(parent)) AS `Association`, f.file_description AS `Description`,f.file_format AS Format,((f.file_size)/1024) AS Size</t>
   </si>
 </sst>
 </file>
@@ -432,22 +426,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="75.81640625" customWidth="1"/>
     <col min="2" max="2" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.81640625" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="40.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.26953125" customWidth="1"/>
+    <col min="4" max="4" width="40.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -455,29 +448,23 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>